<commit_message>
Gridsearch for PLA optimal rewards
</commit_message>
<xml_diff>
--- a/convert_chart.xlsx
+++ b/convert_chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3399CFD-56BD-458B-9FAA-CEA16C082F89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC982CE-B39A-4D14-860E-00CCE92DB0FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -99,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +120,15 @@
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -142,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,6 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +448,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -545,7 +556,7 @@
         <f>C4/B4</f>
         <v>5.18</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -601,14 +612,14 @@
       <c r="C9" s="3">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>5.5</v>
       </c>
       <c r="E9">
         <f>C9/B9</f>
         <v>7.1428571428571432</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>3.9285714285714288</v>
       </c>
@@ -642,7 +653,7 @@
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <v>5.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New visitor attraction model
</commit_message>
<xml_diff>
--- a/convert_chart.xlsx
+++ b/convert_chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC982CE-B39A-4D14-860E-00CCE92DB0FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BE03BE-384A-4C48-A88F-211382D2CD55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>In Reality</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,13 +94,41 @@
   <si>
     <t>time scale</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In reality</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>In simulation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratio</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">random action interval </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB ramp sequence</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ON-OFF </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">observation length </t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +159,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +200,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -460,9 +498,11 @@
     <col min="6" max="6" width="40.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,8 +521,20 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -509,8 +561,23 @@
       <c r="I2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="6">
+        <v>2</v>
+      </c>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6">
+        <f>M2/O2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -538,8 +605,27 @@
       <c r="I3">
         <v>1161</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>15</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>3.75</v>
+      </c>
+      <c r="Q3" s="6" t="e">
+        <f>M3/O3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -560,8 +646,23 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6">
+        <f>M4/O4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -581,8 +682,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="6">
+        <v>4</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6">
+        <f>M5/O5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -602,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -624,7 +740,7 @@
         <v>3.9285714285714288</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
         <v>16</v>
       </c>
@@ -635,7 +751,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G13">
         <v>1</v>
       </c>
@@ -646,7 +762,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G14">
         <v>1</v>
       </c>
@@ -657,7 +773,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G15">
         <v>1</v>
       </c>

</xml_diff>